<commit_message>
actualizacion de documentos de monitoreo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Acciones Correctivas</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Ricardo Novela</t>
   </si>
   <si>
-    <t>Abierto</t>
+    <t>Cerrado</t>
   </si>
   <si>
     <t>Esfuerzos superiores para el área de soporte</t>
@@ -61,17 +61,34 @@
   <si>
     <t>contratar un nuevo elemento en el área de soporte</t>
   </si>
+  <si>
+    <t>Perdidas monetarias tras el cierre del mes de Febrero</t>
+  </si>
+  <si>
+    <t>Solicitar a ventas prestar mas atención en las ventas realizadas</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>Desviación en procesos y productos de venta, implementación y garantia</t>
+  </si>
+  <si>
+    <t>Solicitar a dirección ayuda para requerir apego por el area de ejecución</t>
+  </si>
+  <si>
+    <t>Jovanny Zepda</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$ &quot;* #,##0.00_-;&quot;-$ &quot;* #,##0.00_-;_-&quot;$ &quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,13 +110,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -128,12 +138,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -172,7 +176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,15 +200,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,64 +210,54 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Moneda 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -372,8 +359,8 @@
   </sheetPr>
   <dimension ref="1:29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3519,7 +3506,9 @@
       <c r="H5" s="10" t="n">
         <v>42431</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="n">
+        <v>42431</v>
+      </c>
       <c r="J5" s="9" t="s">
         <v>12</v>
       </c>
@@ -3542,41 +3531,67 @@
       <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="11" t="n">
+      <c r="H6" s="10" t="n">
         <v>42431</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="n">
+        <v>42431</v>
+      </c>
       <c r="J6" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>42433</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>42464</v>
+      </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="9"/>
+      <c r="J7" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>42433</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>42464</v>
+      </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
@@ -3707,170 +3722,170 @@
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="13" t="n">
+      <c r="C18" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="13" t="n">
+      <c r="C19" s="11" t="n">
         <v>15</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="13" t="n">
+      <c r="C20" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="13" t="n">
+      <c r="C21" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="13" t="n">
+      <c r="C23" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="13" t="n">
+      <c r="C24" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="13" t="n">
+      <c r="C25" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="13" t="n">
+      <c r="C26" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="13" t="n">
+      <c r="C27" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="13" t="n">
+      <c r="C28" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="13" t="n">
+      <c r="C29" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
actualicion reporte monitoreo minuta y acciones
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="1:29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3593,7 +3593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="9" t="n">

</xml_diff>

<commit_message>
Reporte de monitores mes de junio
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
@@ -35,7 +35,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Hp EliteBook:</t>
         </r>
@@ -44,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 SI
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Acciones Correctivas</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Desviación en ventas planeadas para el mes de Marzo</t>
   </si>
   <si>
-    <t>En espera de acción correctiva</t>
-  </si>
-  <si>
     <t>Fecha
 Compromiso</t>
   </si>
@@ -159,6 +156,18 @@
   </si>
   <si>
     <t>Presentar esfuerzos superiores a los estimados en la cotización anual de la empresa lo cual provoca perdidas monetarias a la empresa</t>
+  </si>
+  <si>
+    <t>Campaña de publicidad.</t>
+  </si>
+  <si>
+    <t>Tercera campaña de publicidad para Desarrollo y beneficio del CMMi</t>
+  </si>
+  <si>
+    <t>Aplicar la medicion resultante en el CMMi para diferenciar tareas de soporte (implementacion y garantia)</t>
+  </si>
+  <si>
+    <t>En espera de acciones correctivas</t>
   </si>
 </sst>
 </file>
@@ -208,14 +217,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -678,7 +687,7 @@
   <dimension ref="A1:AML29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>2</v>
@@ -3795,16 +3804,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>5</v>
@@ -3984,20 +3993,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" ht="57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="5">
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G11" s="6">
         <v>42468</v>
@@ -4008,25 +4017,27 @@
       <c r="I11" s="7">
         <v>42492</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6">
+        <v>42558</v>
+      </c>
       <c r="K11" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1025" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="5">
         <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G12" s="6">
         <v>42513</v>
@@ -4037,9 +4048,11 @@
       <c r="I12" s="6">
         <v>42521</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6">
+        <v>42558</v>
+      </c>
       <c r="K12" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1025" ht="57" x14ac:dyDescent="0.25">
@@ -4049,13 +4062,13 @@
         <v>9</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G13" s="6">
         <v>42527</v>
@@ -4066,9 +4079,11 @@
       <c r="I13" s="6">
         <v>42528</v>
       </c>
-      <c r="J13" s="6"/>
+      <c r="J13" s="6">
+        <v>42557</v>
+      </c>
       <c r="K13" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1025" ht="114" x14ac:dyDescent="0.25">
@@ -4078,13 +4093,13 @@
         <v>10</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G14" s="6">
         <v>42527</v>
@@ -4095,40 +4110,68 @@
       <c r="I14" s="6">
         <v>42528</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="6">
+        <v>42528</v>
+      </c>
       <c r="K14" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" ht="57" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
         <v>11</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
+      <c r="D15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="6">
+        <v>42557</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="6">
+        <v>42558</v>
+      </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="16" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1025" ht="114" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="5">
         <v>12</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="6">
+        <v>42557</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="6">
+        <v>42558</v>
+      </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
Revision del mes de julio
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Acciones_correctivas_2016.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Acciones Correctivas</t>
   </si>
@@ -687,7 +687,7 @@
   <dimension ref="A1:AML29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,7 +4055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1025" ht="57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1025" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="5">
@@ -4086,7 +4086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1025" ht="114" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1025" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="5">
@@ -4117,7 +4117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1025" ht="57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
@@ -4141,9 +4141,11 @@
       <c r="I15" s="6">
         <v>42558</v>
       </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6">
+        <v>42593</v>
+      </c>
       <c r="K15" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1025" ht="114" x14ac:dyDescent="0.25">
@@ -4152,7 +4154,9 @@
       <c r="C16" s="5">
         <v>12</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
@@ -4173,20 +4177,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="114" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="5">
         <v>13</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="6">
+        <v>42593</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="6">
+        <v>42597</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>

</xml_diff>